<commit_message>
Actualizacion de cosas por hacer
</commit_message>
<xml_diff>
--- a/Meprogramo.xlsx
+++ b/Meprogramo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven Gomez\Documents\Meprogramo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven Gomez\Documents\Meprogramo\Meprogramo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C068FEA3-404E-4ABC-BCD5-6809055BF20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80559547-8DF3-4023-BA63-3C1332976562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="51">
   <si>
     <t>Lunes</t>
   </si>
@@ -167,9 +167,6 @@
     <t>7:00pm Llego a casa/Reposo</t>
   </si>
   <si>
-    <t>7:00pm Llego a casa/Reposo/Toco piano</t>
-  </si>
-  <si>
     <t>//Entrega Lab 1</t>
   </si>
   <si>
@@ -186,6 +183,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Semana 6-11 </t>
+  </si>
+  <si>
+    <t>Vi las clases virtuales</t>
+  </si>
+  <si>
+    <t>Examenes de laboratorio</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -384,18 +387,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -405,10 +406,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -417,12 +418,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -433,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -719,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,9 +772,9 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>35</v>
@@ -792,7 +793,7 @@
       <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -813,8 +814,8 @@
       <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>7</v>
+      <c r="E5" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>32</v>
@@ -834,7 +835,7 @@
       <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="1"/>
@@ -851,26 +852,24 @@
       <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -883,11 +882,11 @@
       <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -900,13 +899,13 @@
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="1"/>
@@ -919,13 +918,13 @@
       <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>26</v>
+      <c r="C11" s="46" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="1"/>
@@ -933,176 +932,165 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="46"/>
+      <c r="D12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="46"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="33"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="A23" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="31" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1110,236 +1098,236 @@
       <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="31" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
+      <c r="B35" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="43"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="33"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="45"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="43" t="s">
+      <c r="D40" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E40" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="45" t="s">
+      <c r="A41" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="45" t="s">
+      <c r="E42" s="43" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="43" t="s">
+      <c r="D43" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="43" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1347,235 +1335,235 @@
       <c r="A44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="47" t="s">
+      <c r="E44" s="45" t="s">
         <v>23</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="43" t="s">
+      <c r="A45" s="13"/>
+      <c r="B45" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="45" t="s">
+      <c r="E45" s="43" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="43" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="43" t="s">
+      <c r="D46" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="45" t="s">
+      <c r="E46" s="43" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D47" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="45"/>
+      <c r="E47" s="43"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="48" t="s">
+      <c r="A48" s="13"/>
+      <c r="B48" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="41"/>
+      <c r="E49" s="43"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="48"/>
+      <c r="B53" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" s="49" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="43"/>
-      <c r="E49" s="45"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" s="45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="53" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="B56" s="55"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="56"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54"/>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="49"/>
+      <c r="A57" s="55"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="47"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="43" t="s">
+      <c r="A58" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="43" t="s">
+      <c r="D58" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="49" t="s">
+      <c r="E58" s="47" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" s="49" t="s">
+      <c r="A59" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="47" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="57" t="s">
+      <c r="A60" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="48" t="s">
+      <c r="C60" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="43" t="s">
+      <c r="D60" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="47" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B61" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="48" t="s">
+      <c r="C61" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="43" t="s">
+      <c r="D61" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E61" s="49" t="s">
+      <c r="E61" s="47" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1583,149 +1571,149 @@
       <c r="A62" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="43" t="s">
+      <c r="D62" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E62" s="61" t="s">
+      <c r="E62" s="59" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
-      <c r="B63" s="43" t="s">
+      <c r="A63" s="55"/>
+      <c r="B63" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="48" t="s">
+      <c r="C63" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="49" t="s">
+      <c r="E63" s="47" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
-      <c r="B64" s="43" t="s">
+      <c r="A64" s="55"/>
+      <c r="B64" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="48" t="s">
+      <c r="C64" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D64" s="43" t="s">
+      <c r="D64" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="E64" s="49" t="s">
+      <c r="E64" s="47" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="57" t="s">
+      <c r="A65" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="43" t="s">
+      <c r="D65" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="49"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="57"/>
-      <c r="B66" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E66" s="12" t="s">
+      <c r="A66" s="55"/>
+      <c r="B66" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="57"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="11" t="s">
+      <c r="A67" s="55"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="43"/>
-      <c r="E67" s="49"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="47"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="57" t="s">
+      <c r="A68" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="48" t="s">
+      <c r="C68" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D68" s="43" t="s">
+      <c r="D68" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="E68" s="49" t="s">
+      <c r="E68" s="47" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="57" t="s">
+      <c r="A69" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="48" t="s">
+      <c r="C69" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="43" t="s">
+      <c r="D69" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="49" t="s">
+      <c r="E69" s="47" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D70" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="49" t="s">
+      <c r="A70" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="47" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="58"/>
-      <c r="B71" s="51" t="s">
+      <c r="A71" s="56"/>
+      <c r="B71" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="51" t="s">
+      <c r="D71" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E71" s="62" t="s">
+      <c r="E71" s="60" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actilazacion de tareas por hacer
</commit_message>
<xml_diff>
--- a/Meprogramo.xlsx
+++ b/Meprogramo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven Gomez\Documents\Meprogramo\Meprogramo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80559547-8DF3-4023-BA63-3C1332976562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D2E8F-2802-4961-979A-D959F9A457BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="53">
   <si>
     <t>Lunes</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Examenes de laboratorio</t>
+  </si>
+  <si>
+    <t>Avanzar con el lab1 de digitales</t>
+  </si>
+  <si>
+    <t>Entregar la tarea del lab de info2</t>
   </si>
 </sst>
 </file>
@@ -721,7 +727,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +954,9 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="46"/>
+      <c r="C13" s="46" t="s">
+        <v>51</v>
+      </c>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,7 +981,9 @@
       <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="D15" s="10" t="s">
         <v>18</v>
       </c>

</xml_diff>